<commit_message>
Added point and polygon
Need to fix comparePoly() for Polygon.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EAF4D4-C315-4CB0-8EA6-C89EBF4D40F6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67EC674-1868-47E6-8443-E7CBA4FDAE82}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t>Sunday 8.8.18</t>
+  </si>
+  <si>
+    <t>Monday 9.9.18</t>
+  </si>
+  <si>
+    <t>0900-1100</t>
+  </si>
+  <si>
+    <t>Setting up repo on laptop + building simple classes</t>
   </si>
 </sst>
 </file>
@@ -118,13 +127,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A90FC5F8-4544-4D0D-9FA4-F5678436F556}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A90FC5F8-4544-4D0D-9FA4-F5678436F556}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A1:D32" xr:uid="{8FFAF145-D05C-4D40-85F8-11DC3C07801E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A6C54378-A635-4BFE-9A30-6C0546A6B7A5}" name="Date" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{D6724FE4-E1F3-48D5-A850-5C81059B21DE}" name="Time" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{90392D3D-45AB-4259-98B7-C74468C43BA0}" name="Hours" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C46D515F-1A63-4F6F-B036-71F4FE15781A}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A6C54378-A635-4BFE-9A30-6C0546A6B7A5}" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D6724FE4-E1F3-48D5-A850-5C81059B21DE}" name="Time" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{90392D3D-45AB-4259-98B7-C74468C43BA0}" name="Hours" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C46D515F-1A63-4F6F-B036-71F4FE15781A}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -395,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,10 +445,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -616,7 +633,7 @@
       </c>
       <c r="C32" s="1">
         <f>SUBTOTAL(109,C2:C31)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added formatted toStrings( ) for Point and Polygon
Still need to sort out a comparePoly thing...
Next thing I will do is make PlanarShapes
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67EC674-1868-47E6-8443-E7CBA4FDAE82}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5821F87E-8487-44B4-B9AB-CB86C21B0ED6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>Setting up repo on laptop + building simple classes</t>
+  </si>
+  <si>
+    <t>Tuesday 10.4.18</t>
+  </si>
+  <si>
+    <t>2200-2300</t>
+  </si>
+  <si>
+    <t>Completing Point and Polygon</t>
   </si>
 </sst>
 </file>
@@ -405,7 +414,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +468,18 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -633,7 +650,7 @@
       </c>
       <c r="C32" s="1">
         <f>SUBTOTAL(109,C2:C31)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
added some hours to time track
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5821F87E-8487-44B4-B9AB-CB86C21B0ED6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAC0711-85ED-4E1D-B591-D77B9722E13F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
     <t>2200-2300</t>
   </si>
   <si>
-    <t>Completing Point and Polygon</t>
+    <t>Completing Point and Polygon + Reading about polymorphism</t>
   </si>
 </sst>
 </file>
@@ -414,7 +414,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Setup MyPolygons have not tested it though, must implement main
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAC0711-85ED-4E1D-B591-D77B9722E13F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747252A5-4E70-4F1F-8CD2-EDB8831B6593}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>Completing Point and Polygon + Reading about polymorphism</t>
+  </si>
+  <si>
+    <t>Monday 16.4.18</t>
+  </si>
+  <si>
+    <t>1630 - 1830</t>
+  </si>
+  <si>
+    <t>Rewriting assignment one in Java</t>
   </si>
 </sst>
 </file>
@@ -414,7 +423,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B4" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,10 +491,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -650,7 +667,7 @@
       </c>
       <c r="C32" s="1">
         <f>SUBTOTAL(109,C2:C31)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Implementing main program. Need to fix reader/sorter etc.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747252A5-4E70-4F1F-8CD2-EDB8831B6593}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FD93DD-A4A7-4ED8-B1BC-3CAADB4843CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Rewriting assignment one in Java</t>
+  </si>
+  <si>
+    <t>Tuesday 17.4.18</t>
+  </si>
+  <si>
+    <t>1030 - 1130</t>
+  </si>
+  <si>
+    <t>Implementing LinkedList</t>
   </si>
 </sst>
 </file>
@@ -423,7 +432,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B3:B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,10 +514,18 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -667,7 +684,7 @@
       </c>
       <c r="C32" s="1">
         <f>SUBTOTAL(109,C2:C31)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Got ComparePoly Interface working
Need to get sorting working inside the subclass "SortedPolygons".
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FD93DD-A4A7-4ED8-B1BC-3CAADB4843CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128B5C48-15EA-4B33-932E-87CFFD1476D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -80,6 +80,21 @@
   </si>
   <si>
     <t>Implementing LinkedList</t>
+  </si>
+  <si>
+    <t>Monday 23.4.18</t>
+  </si>
+  <si>
+    <t>1200-1500</t>
+  </si>
+  <si>
+    <t>Theory + interface (ComparePolygons) + subclass (SortedPolygons)</t>
+  </si>
+  <si>
+    <t>1630-1730</t>
+  </si>
+  <si>
+    <t>Getting comparePolygons to work</t>
   </si>
 </sst>
 </file>
@@ -432,7 +447,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,16 +543,32 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -684,7 +715,7 @@
       </c>
       <c r="C32" s="1">
         <f>SUBTOTAL(109,C2:C31)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Insertion Sort works my god.
it works
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128B5C48-15EA-4B33-932E-87CFFD1476D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE21258E-588F-46DD-ACBB-1E9239BC665B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -95,6 +95,18 @@
   </si>
   <si>
     <t>Getting comparePolygons to work</t>
+  </si>
+  <si>
+    <t>Sunday 29.4.18</t>
+  </si>
+  <si>
+    <t>Insertion Sort</t>
+  </si>
+  <si>
+    <t>Saturday 28.4.18</t>
+  </si>
+  <si>
+    <t>2300-0100</t>
   </si>
 </sst>
 </file>
@@ -447,7 +459,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,16 +583,32 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -715,7 +743,7 @@
       </c>
       <c r="C32" s="1">
         <f>SUBTOTAL(109,C2:C31)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Got comparable working, interfaces etc.
Need to make iteration work and shapesfactory thing.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAC0711-85ED-4E1D-B591-D77B9722E13F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB383299-6055-4058-AC53-CF2D3FE6337A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,63 @@
   </si>
   <si>
     <t>Completing Point and Polygon + Reading about polymorphism</t>
+  </si>
+  <si>
+    <t>Monday 16.4.18</t>
+  </si>
+  <si>
+    <t>1630 - 1830</t>
+  </si>
+  <si>
+    <t>Rewriting assignment one in Java</t>
+  </si>
+  <si>
+    <t>Tuesday 17.4.18</t>
+  </si>
+  <si>
+    <t>1030 - 1130</t>
+  </si>
+  <si>
+    <t>Implementing LinkedList</t>
+  </si>
+  <si>
+    <t>Monday 23.4.18</t>
+  </si>
+  <si>
+    <t>1200-1500</t>
+  </si>
+  <si>
+    <t>Theory + interface (ComparePolygons) + subclass (SortedPolygons)</t>
+  </si>
+  <si>
+    <t>1630-1730</t>
+  </si>
+  <si>
+    <t>Getting comparePolygons to work</t>
+  </si>
+  <si>
+    <t>Sunday 29.4.18</t>
+  </si>
+  <si>
+    <t>Insertion Sort</t>
+  </si>
+  <si>
+    <t>Saturday 28.4.18</t>
+  </si>
+  <si>
+    <t>2300-0100</t>
+  </si>
+  <si>
+    <t>1200-1730</t>
+  </si>
+  <si>
+    <t>Insertion Sort Works</t>
+  </si>
+  <si>
+    <t>Sunday 29.4.1.8</t>
+  </si>
+  <si>
+    <t>Comparable Interfaces</t>
   </si>
 </sst>
 </file>
@@ -414,7 +471,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,46 +539,102 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -650,7 +763,7 @@
       </c>
       <c r="C32" s="1">
         <f>SUBTOTAL(109,C2:C31)</f>
-        <v>4</v>
+        <v>21.5</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Got reader going good with Scanner class.
Love that Scanner class I do.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8839CC-D2D4-4156-BF00-AE60755FE559}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AD8C8B-0CEE-4F15-AA66-71706BFD8A07}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Iterator and Improved Reader</t>
+  </si>
+  <si>
+    <t>1600-1700</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,9 +663,15 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -780,7 +789,7 @@
       </c>
       <c r="C32" s="1">
         <f>SUBTOTAL(109,C2:C31)</f>
-        <v>23.5</v>
+        <v>24.5</v>
       </c>
       <c r="D32" s="1"/>
     </row>

</xml_diff>

<commit_message>
Finished my dude. Well done.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AD8C8B-0CEE-4F15-AA66-71706BFD8A07}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A039E9EB-DB05-4D20-8C8C-93DC2132F6C2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -131,14 +131,40 @@
   </si>
   <si>
     <t>1600-1700</t>
+  </si>
+  <si>
+    <t>2100-2300</t>
+  </si>
+  <si>
+    <t>Shapes factory</t>
+  </si>
+  <si>
+    <t>Circle + Semicircle</t>
+  </si>
+  <si>
+    <t>Sunday 6.5.18</t>
+  </si>
+  <si>
+    <t>1200-1600</t>
+  </si>
+  <si>
+    <t>Report and Polishing of code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -166,9 +192,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -205,8 +234,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A90FC5F8-4544-4D0D-9FA4-F5678436F556}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="A1:D32" xr:uid="{8FFAF145-D05C-4D40-85F8-11DC3C07801E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A90FC5F8-4544-4D0D-9FA4-F5678436F556}" name="Table1" displayName="Table1" ref="A1:D16" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:D16" xr:uid="{8FFAF145-D05C-4D40-85F8-11DC3C07801E}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A6C54378-A635-4BFE-9A30-6C0546A6B7A5}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{D6724FE4-E1F3-48D5-A850-5C81059B21DE}" name="Time" dataDxfId="2"/>
@@ -480,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,131 +701,54 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2">
+        <f>SUBTOTAL(109,C2:C15)</f>
+        <v>30.5</v>
+      </c>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="1">
-        <f>SUBTOTAL(109,C2:C31)</f>
-        <v>24.5</v>
-      </c>
-      <c r="D32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>